<commit_message>
advanced post survey data
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_EndofCampIntro_Likert.xlsx
+++ b/Data/GGEE_23_EndofCampIntro_Likert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviarandell/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34650173-6CE9-3748-B692-696482D9A32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F4829-2848-5D49-A4C0-020801F71F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="500" windowWidth="13380" windowHeight="15760" firstSheet="4" activeTab="6" xr2:uid="{7292BB22-2922-0840-9871-47BBFB9FAADB}"/>
+    <workbookView xWindow="15420" yWindow="500" windowWidth="13380" windowHeight="15760" firstSheet="5" activeTab="7" xr2:uid="{7292BB22-2922-0840-9871-47BBFB9FAADB}"/>
   </bookViews>
   <sheets>
     <sheet name="Prior Experience Raw" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Post Skill level Raw" sheetId="5" r:id="rId5"/>
     <sheet name="Post Skill Level Likert" sheetId="6" r:id="rId6"/>
     <sheet name="Confidence Raw" sheetId="8" r:id="rId7"/>
+    <sheet name="Confidence Likert" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="26">
   <si>
     <t>A lot of experience</t>
   </si>
@@ -119,6 +120,9 @@
   </si>
   <si>
     <t>Somewhat disagree</t>
+  </si>
+  <si>
+    <t>I felt confident when completing today's camp activities.</t>
   </si>
 </sst>
 </file>
@@ -2948,702 +2952,848 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FCA4F8-9DF8-024F-958E-6AE6F1B5BA34}">
-  <dimension ref="A1:A138"/>
+  <dimension ref="A1:E138"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF(A2:A138, "Strongly agree" )</f>
+        <v>78</v>
+      </c>
+      <c r="E2">
+        <f>D2/D7*100</f>
+        <v>56.934306569343065</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <f>COUNTIF(A2:A138, "Somewhat agree")</f>
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <f>D3/D7*100</f>
+        <v>28.467153284671532</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIF(A2:A138, "Neither agree nor disagree")</f>
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <f>D4/D7*100</f>
+        <v>8.0291970802919703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <f>COUNTIF(A2:A138, "Somewhat disagree")</f>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>D5/D7*100</f>
+        <v>2.9197080291970803</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <f>COUNTIF(A2:A138, "Strongly disagree")</f>
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f>D6/D7*100</f>
+        <v>3.6496350364963499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DF5BBD-4BF0-2F41-A50A-92346DB2EC06}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A138"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>78</v>
+      </c>
+      <c r="E7">
+        <v>56.934306569343065</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>28.467153284671532</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>8.0291970802919703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>2.9197080291970803</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>20</v>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>3.6496350364963499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>